<commit_message>
Update - Numbers.py and Database.py
</commit_message>
<xml_diff>
--- a/DataBase/Usuarios.xlsx
+++ b/DataBase/Usuarios.xlsx
@@ -507,21 +507,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>If they had finished their work earlier, they could have gone to the party.</t>
+          <t>One rainy afternoon, Emily's beloved teddy bear went missing. Frantically, she searched every corner of her room, but the bear was nowhere to be found. With tears in her eyes, Emily ventured outside into the downpour, determined to find her lost friend. As she wandered through the streets, she spotted a familiar sight - a soggy teddy bear lying abandoned on a bench. With a joyful cry, Emily rushed forward and scooped up her precious bear. Grateful and relieved, she hugged her teddy tightly, knowing that some bonds are unbreakable, even in the stormiest of times.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Se eles tivessem terminado o trabalho mais cedo, eles poderiam ter ido à festa.</t>
+          <t>Em uma tarde chuvosa, o amado urso de pelúcia de Emily desapareceu. Desesperadamente, ela procurou em todos os cantos do seu quarto, mas o urso não estava em lugar nenhum. Com lágrimas nos olhos, Emily aventurou-se do lado de fora sob a chuva forte, determinada a encontrar seu amigo perdido. Enquanto vagava pelas ruas, ela avistou uma visão familiar - um urso de pelúcia encharcado deitado abandonado em um banco. Com um grito alegre, Emily correu para frente e pegou seu urso precioso. Grata e aliviada, ela abraçou seu urso com força, sabendo que alguns laços são inquebráveis, mesmo nos tempos mais tempestuosos.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Intermediário</t>
+          <t>Básico Avançado</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>86</v>
+        <v>250</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Add the folder FrasesHistoprias and clean code
</commit_message>
<xml_diff>
--- a/DataBase/Usuarios.xlsx
+++ b/DataBase/Usuarios.xlsx
@@ -507,21 +507,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>One rainy afternoon, Emily's beloved teddy bear went missing. Frantically, she searched every corner of her room, but the bear was nowhere to be found. With tears in her eyes, Emily ventured outside into the downpour, determined to find her lost friend. As she wandered through the streets, she spotted a familiar sight - a soggy teddy bear lying abandoned on a bench. With a joyful cry, Emily rushed forward and scooped up her precious bear. Grateful and relieved, she hugged her teddy tightly, knowing that some bonds are unbreakable, even in the stormiest of times.</t>
+          <t>In a dusty old attic, Emily found a magical paintbrush hidden among the cobwebs. With each stroke, the paintbrush brought her drawings to life. She painted colorful landscapes and majestic creatures that danced off the page. Excitedly, Emily shared her creations with her friends and family, filling their lives with wonder and joy. But one day, she realized that her brush could also mend broken hearts and heal old wounds. From that day on, Emily used her gift to spread love and happiness wherever she went, proving that sometimes the most magical things are found in the simplest of places.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Em uma tarde chuvosa, o amado urso de pelúcia de Emily desapareceu. Desesperadamente, ela procurou em todos os cantos do seu quarto, mas o urso não estava em lugar nenhum. Com lágrimas nos olhos, Emily aventurou-se do lado de fora sob a chuva forte, determinada a encontrar seu amigo perdido. Enquanto vagava pelas ruas, ela avistou uma visão familiar - um urso de pelúcia encharcado deitado abandonado em um banco. Com um grito alegre, Emily correu para frente e pegou seu urso precioso. Grata e aliviada, ela abraçou seu urso com força, sabendo que alguns laços são inquebráveis, mesmo nos tempos mais tempestuosos.</t>
+          <t>Em um sótão empoeirado, Emily encontrou um pincel mágico escondido entre as teias de aranha. Com cada traço, o pincel trazia suas desenhos à vida. Ela pintava paisagens coloridas e criaturas majestosas que dançavam fora da página. Animada, Emily compartilhava suas criações com seus amigos e família, enchendo suas vidas de admiração e alegria. Mas um dia, ela percebeu que seu pincel também podia consertar corações partidos e curar velhas feridas. A partir desse dia, Emily usou seu dom para espalhar amor e felicidade por onde passava, provando que às vezes as coisas mais mágicas são encontradas nos lugares mais simples.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Básico Avançado</t>
+          <t>Básico</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>250</v>
+        <v>609</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -530,7 +530,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Frase</t>
+          <t>Aprender</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Update - Add Alphabet Pronunciation
</commit_message>
<xml_diff>
--- a/DataBase/Usuarios.xlsx
+++ b/DataBase/Usuarios.xlsx
@@ -507,12 +507,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>She is a good singer.</t>
+          <t>Amy and her family are going on a picnic. They pack sandwiches, fruits, and drinks in a basket. Amy helps her mom make the sandwiches. They also bring a blanket to sit on. When they arrive at the park, Amy and her brother play tag while their parents set up the picnic. They all enjoy the delicious food and the beautiful weather.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Ela é uma boa cantora.</t>
+          <t>Amy e sua família vão fazer um piquenique. Eles preparam sanduíches, frutas e bebidas em uma cesta. Amy ajuda sua mãe a fazer os sanduíches. Eles também trazem um cobertor para sentar. Quando chegam ao parque, Amy e seu irmão brincam de pega enquanto seus pais arrumam o piquenique. Todos aproveitam a comida deliciosa e o clima agradável.</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -521,11 +521,11 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>9</v>
+        <v>73</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>/Aprender</t>
+          <t>/OK</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">

</xml_diff>

<commit_message>
Update - Code Documentation
</commit_message>
<xml_diff>
--- a/DataBase/Usuarios.xlsx
+++ b/DataBase/Usuarios.xlsx
@@ -447,10 +447,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -500,6 +500,11 @@
           <t>Frases  / Aprender</t>
         </is>
       </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Letra</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -521,7 +526,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>73</v>
+        <v>16</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -531,6 +536,11 @@
       <c r="G2" t="inlineStr">
         <is>
           <t>Aprender</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Q</t>
         </is>
       </c>
     </row>

</xml_diff>